<commit_message>
i created my project
</commit_message>
<xml_diff>
--- a/data/mydata.xlsx
+++ b/data/mydata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulvihuseynov/Desktop/20080109/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F16346-9AEC-1446-9428-27ABA60E3BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103C2824-7679-374E-9040-4234E7CEB0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -752,7 +752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>